<commit_message>
Esthétisme et petites modifications
</commit_message>
<xml_diff>
--- a/equipe4-excel.xlsx
+++ b/equipe4-excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\ATCR-TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Analyse et traitement collectif du risque\Calcul-prestations\ATCR-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C42F820-3876-47FB-834D-387067B2F9AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF01B3-858F-4E7F-A4C8-97FC1B0C75A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTION 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="QUESTION 6" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,11 +30,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1628,7 @@
     <col min="3" max="3" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="5"/>
     <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="10.85546875" style="1"/>
     <col min="11" max="11" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3073,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A40" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4575,8 +4575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,7 +4595,8 @@
     <col min="13" max="13" width="49.42578125" style="1" customWidth="1"/>
     <col min="14" max="16" width="10.85546875" style="1"/>
     <col min="17" max="17" width="43.85546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.85546875" style="1"/>
+    <col min="18" max="18" width="12.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4633,11 +4634,11 @@
         <v>64</v>
       </c>
       <c r="D3" s="85">
-        <f t="shared" ref="D3:D6" si="0">D4*(1+$N$6)</f>
+        <f t="shared" ref="D3:E7" si="0">D4*(1+$N$6)</f>
         <v>54360.857384573552</v>
       </c>
       <c r="E3" s="30">
-        <f t="shared" ref="E3:E6" si="1">E4*(1+$N$6)</f>
+        <f t="shared" si="0"/>
         <v>65738.689948352316</v>
       </c>
       <c r="F3" s="125">
@@ -4671,11 +4672,11 @@
         <v>52905.943926592263</v>
       </c>
       <c r="E4" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>63979.260290367209</v>
       </c>
       <c r="G4" s="90">
-        <f t="shared" ref="G4:G66" si="2">D4*($N$9/E4)</f>
+        <f t="shared" ref="G4:G66" si="1">D4*($N$9/E4)</f>
         <v>52944.888948161155</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -4705,15 +4706,15 @@
         <v>62</v>
       </c>
       <c r="D5" s="85">
-        <f t="shared" si="0"/>
+        <f>D6*(1+$N$6)</f>
         <v>51489.969758240644</v>
       </c>
       <c r="E5" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>62266.919990625014</v>
       </c>
       <c r="G5" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>52944.888948161162</v>
       </c>
       <c r="I5" s="12" t="s">
@@ -4745,15 +4746,15 @@
         <v>61</v>
       </c>
       <c r="D6" s="85">
-        <f t="shared" si="0"/>
+        <f>D7*(1+$N$6)</f>
         <v>50111.892708750012</v>
       </c>
       <c r="E6" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60600.40875000001</v>
       </c>
       <c r="G6" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>52944.888948161162</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -4789,11 +4790,11 @@
         <v>48770.698500000006</v>
       </c>
       <c r="E7" s="30">
-        <f>E8*(1+$N$6)</f>
+        <f t="shared" si="0"/>
         <v>58978.500000000007</v>
       </c>
       <c r="G7" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>52944.888948161155</v>
       </c>
       <c r="I7" s="12" t="s">
@@ -4830,7 +4831,7 @@
         <v>57400</v>
       </c>
       <c r="G8" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>52944.888948161148</v>
       </c>
       <c r="I8" s="12" t="s">
@@ -4872,7 +4873,7 @@
         <v>55863.746958637465</v>
       </c>
       <c r="G9" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>53490.398525712815</v>
       </c>
       <c r="I9" s="13" t="s">
@@ -4907,11 +4908,11 @@
         <v>46323.45</v>
       </c>
       <c r="E10" s="81">
-        <f t="shared" ref="E10:E67" si="3">E9/(1.0275)</f>
+        <f t="shared" ref="E10:E67" si="2">E9/(1.0275)</f>
         <v>54368.610178722593</v>
       </c>
       <c r="G10" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>54552.09757942929</v>
       </c>
       <c r="I10" s="11" t="s">
@@ -4947,11 +4948,11 @@
         <v>45538.98</v>
       </c>
       <c r="E11" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>52913.489225034151</v>
       </c>
       <c r="G11" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55103.056224114152</v>
       </c>
       <c r="I11" s="13" t="s">
@@ -4980,11 +4981,11 @@
         <v>44665.14</v>
       </c>
       <c r="E12" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>51497.313114388468</v>
       </c>
       <c r="G12" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55531.9492882048</v>
       </c>
       <c r="M12" s="12" t="s">
@@ -5007,11 +5008,11 @@
         <v>43811.159999999996</v>
       </c>
       <c r="E13" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50119.039527385365</v>
       </c>
       <c r="G13" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55968.130650666404</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -5036,11 +5037,11 @@
         <v>42699</v>
       </c>
       <c r="E14" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>48777.654041250957</v>
       </c>
       <c r="G14" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>56047.414607277169</v>
       </c>
       <c r="M14" s="12" t="s">
@@ -5061,11 +5062,11 @@
         <v>42291.87</v>
       </c>
       <c r="E15" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>47472.169383212604</v>
       </c>
       <c r="G15" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57039.616774356829</v>
       </c>
       <c r="M15" s="13" t="s">
@@ -5090,11 +5091,11 @@
         <v>41576.909999999996</v>
       </c>
       <c r="E16" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46201.624703856542</v>
       </c>
       <c r="G16" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57617.412422792535</v>
       </c>
       <c r="M16" s="122" t="s">
@@ -5119,11 +5120,11 @@
         <v>40812.300000000003</v>
       </c>
       <c r="E17" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44965.084869933373</v>
       </c>
       <c r="G17" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>58113.153354851558</v>
       </c>
       <c r="M17" s="54"/>
@@ -5143,11 +5144,11 @@
         <v>40137.06</v>
       </c>
       <c r="E18" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>43761.639776090873</v>
       </c>
       <c r="G18" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>58723.341465077501</v>
       </c>
       <c r="M18" s="126" t="s">
@@ -5166,11 +5167,11 @@
         <v>39620.699999999997</v>
       </c>
       <c r="E19" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>42590.403675027614</v>
       </c>
       <c r="G19" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>59561.986909429696</v>
       </c>
       <c r="M19" s="11" t="s">
@@ -5189,11 +5190,11 @@
         <v>38766.720000000001</v>
       </c>
       <c r="E20" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>41450.514525574319</v>
       </c>
       <c r="G20" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>59880.845064914771</v>
       </c>
       <c r="M20" s="12" t="s">
@@ -5212,11 +5213,11 @@
         <v>37882.949999999997</v>
       </c>
       <c r="E21" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>40341.133358223182</v>
       </c>
       <c r="G21" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60124.916260379796</v>
       </c>
       <c r="M21" s="12"/>
@@ -5233,11 +5234,11 @@
         <v>37336.800000000003</v>
       </c>
       <c r="E22" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>39261.443657638127</v>
       </c>
       <c r="G22" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60887.706810052783</v>
       </c>
       <c r="M22" s="12" t="s">
@@ -5256,11 +5257,11 @@
         <v>36403.379999999997</v>
       </c>
       <c r="E23" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>38210.650761691606</v>
       </c>
       <c r="G23" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60998.065778645992</v>
       </c>
       <c r="M23" s="12" t="s">
@@ -5279,11 +5280,11 @@
         <v>34755</v>
       </c>
       <c r="E24" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>37187.981276585502</v>
       </c>
       <c r="G24" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>59837.505198160303</v>
       </c>
       <c r="M24" s="12"/>
@@ -5300,11 +5301,11 @@
         <v>34546.47</v>
       </c>
       <c r="E25" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>36192.682507625788</v>
       </c>
       <c r="G25" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>61114.138371563065</v>
       </c>
       <c r="M25" s="12" t="s">
@@ -5323,11 +5324,11 @@
         <v>33920.879999999997</v>
       </c>
       <c r="E26" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>35224.021905231908</v>
       </c>
       <c r="G26" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>61657.648415028474</v>
       </c>
       <c r="M26" s="12"/>
@@ -5344,11 +5345,11 @@
         <v>32769</v>
       </c>
       <c r="E27" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>34281.286525773146</v>
       </c>
       <c r="G27" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>61201.894427183201</v>
       </c>
       <c r="M27" s="56" t="s">
@@ -5367,11 +5368,11 @@
         <v>32351.94</v>
       </c>
       <c r="E28" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>33363.782506835174</v>
       </c>
       <c r="G28" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>62084.592659080721</v>
       </c>
       <c r="M28" s="54"/>
@@ -5388,11 +5389,11 @@
         <v>31155.375</v>
       </c>
       <c r="E29" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>32470.834556530579</v>
       </c>
       <c r="G29" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>61432.518639727467</v>
       </c>
     </row>
@@ -5407,11 +5408,11 @@
         <v>0</v>
       </c>
       <c r="E30" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>31601.785456477446</v>
       </c>
       <c r="G30" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M30" s="126" t="s">
@@ -5430,11 +5431,11 @@
         <v>1492</v>
       </c>
       <c r="E31" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>30755.995578080237</v>
       </c>
       <c r="G31" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3105.9740457832272</v>
       </c>
       <c r="M31" s="77" t="s">
@@ -5456,11 +5457,11 @@
         <v>1302</v>
       </c>
       <c r="E32" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>29932.842411756919</v>
       </c>
       <c r="G32" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2784.9782897580635</v>
       </c>
       <c r="M32" s="78" t="s">
@@ -5482,11 +5483,11 @@
         <v>0</v>
       </c>
       <c r="E33" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>29131.720108765858</v>
       </c>
       <c r="G33" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M33" s="79" t="s">
@@ -5508,11 +5509,11 @@
         <v>0</v>
       </c>
       <c r="E34" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>28352.039035295238</v>
       </c>
       <c r="G34" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M34" s="54"/>
@@ -5529,11 +5530,11 @@
         <v>0</v>
       </c>
       <c r="E35" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>27593.225338486849</v>
       </c>
       <c r="G35" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M35" s="54"/>
@@ -5550,11 +5551,11 @@
         <v>0</v>
       </c>
       <c r="E36" s="83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>26854.72052407479</v>
       </c>
       <c r="G36" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5569,11 +5570,11 @@
         <v>24854.79</v>
       </c>
       <c r="E37" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>26135.981045328259</v>
       </c>
       <c r="G37" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60887.771708566332</v>
       </c>
     </row>
@@ -5588,11 +5589,11 @@
         <v>24825</v>
       </c>
       <c r="E38" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>25436.47790299587</v>
       </c>
       <c r="G38" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>62487.200789604387</v>
       </c>
     </row>
@@ -5607,11 +5608,11 @@
         <v>22789.35</v>
       </c>
       <c r="E39" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>24755.696255957049</v>
       </c>
       <c r="G39" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>58940.739708790381</v>
       </c>
     </row>
@@ -5626,11 +5627,11 @@
         <v>22243.200000000001</v>
       </c>
       <c r="E40" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>24093.135042293965</v>
       </c>
       <c r="G40" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>59110.242489652272</v>
       </c>
     </row>
@@ -5645,11 +5646,11 @@
         <v>20853</v>
       </c>
       <c r="E41" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>23448.306610505075</v>
       </c>
       <c r="G41" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>56939.788273235361</v>
       </c>
     </row>
@@ -5664,11 +5665,11 @@
         <v>19860</v>
       </c>
       <c r="E42" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>22820.736360588879</v>
       </c>
       <c r="G42" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55719.649953094602</v>
       </c>
     </row>
@@ -5683,11 +5684,11 @@
         <v>0</v>
       </c>
       <c r="E43" s="84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>22209.962394733699</v>
       </c>
       <c r="G43" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5702,11 +5703,11 @@
         <v>0</v>
       </c>
       <c r="E44" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21615.535177356396</v>
       </c>
       <c r="G44" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5721,11 +5722,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21037.017204239801</v>
       </c>
       <c r="G45" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5740,11 +5741,11 @@
         <v>0</v>
       </c>
       <c r="E46" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20473.982680525351</v>
       </c>
       <c r="G46" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5759,11 +5760,11 @@
         <v>0</v>
       </c>
       <c r="E47" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19926.017207323941</v>
       </c>
       <c r="G47" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5778,11 +5779,11 @@
         <v>0</v>
       </c>
       <c r="E48" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19392.717476714297</v>
       </c>
       <c r="G48" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5797,11 +5798,11 @@
         <v>0</v>
       </c>
       <c r="E49" s="82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18873.690974904424</v>
       </c>
       <c r="G49" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5816,11 +5817,11 @@
         <v>0</v>
       </c>
       <c r="E50" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18368.555693337639</v>
       </c>
       <c r="G50" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5835,11 +5836,11 @@
         <v>0</v>
       </c>
       <c r="E51" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17876.939847530546</v>
       </c>
       <c r="G51" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5854,11 +5855,11 @@
         <v>0</v>
       </c>
       <c r="E52" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17398.481603436052</v>
       </c>
       <c r="G52" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5873,11 +5874,11 @@
         <v>0</v>
       </c>
       <c r="E53" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16932.828811129977</v>
       </c>
       <c r="G53" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5892,11 +5893,11 @@
         <v>0</v>
       </c>
       <c r="E54" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16479.638745625281</v>
       </c>
       <c r="G54" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5911,11 +5912,11 @@
         <v>0</v>
       </c>
       <c r="E55" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16038.577854623143</v>
       </c>
       <c r="G55" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5930,11 +5931,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15609.321513015224</v>
       </c>
       <c r="G56" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5949,11 +5950,11 @@
         <v>0</v>
       </c>
       <c r="E57" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15191.55378395642</v>
       </c>
       <c r="G57" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5968,11 +5969,11 @@
         <v>0</v>
       </c>
       <c r="E58" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14784.967186332282</v>
       </c>
       <c r="G58" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5987,11 +5988,11 @@
         <v>0</v>
       </c>
       <c r="E59" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14389.262468449908</v>
       </c>
       <c r="G59" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6006,11 +6007,11 @@
         <v>0</v>
       </c>
       <c r="E60" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14004.148387785797</v>
       </c>
       <c r="G60" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6025,11 +6026,11 @@
         <v>0</v>
       </c>
       <c r="E61" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>13629.341496628513</v>
       </c>
       <c r="G61" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6044,11 +6045,11 @@
         <v>0</v>
       </c>
       <c r="E62" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>13264.565933458405</v>
       </c>
       <c r="G62" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6063,11 +6064,11 @@
         <v>0</v>
       </c>
       <c r="E63" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12909.553219910855</v>
       </c>
       <c r="G63" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6082,11 +6083,11 @@
         <v>0</v>
       </c>
       <c r="E64" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12564.04206317358</v>
       </c>
       <c r="G64" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6101,11 +6102,11 @@
         <v>0</v>
       </c>
       <c r="E65" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12227.778163672583</v>
       </c>
       <c r="G65" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6120,11 +6121,11 @@
         <v>0</v>
       </c>
       <c r="E66" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11900.51402790519</v>
       </c>
       <c r="G66" s="90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6139,7 +6140,7 @@
         <v>0</v>
       </c>
       <c r="E67" s="81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11582.008786282422</v>
       </c>
     </row>
@@ -6157,8 +6158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="74" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>